<commit_message>
Updated json schema to include yh_symbol in each dict. This is to make it easier to store the data in sql format. Also, required fields were added for the same reason, they will form the unique indices when storing the data to sql or mongodb.
Tests were updated accordingly.
</commit_message>
<xml_diff>
--- a/financejson/tests/test.xlsx
+++ b/financejson/tests/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>symbol</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>US_XYZ</t>
+  </si>
+  <si>
+    <t>index_symbol</t>
   </si>
   <si>
     <t>currency</t>
@@ -506,27 +509,33 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -535,18 +544,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -560,24 +569,30 @@
       <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5</v>
       </c>
     </row>
@@ -611,22 +626,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -634,22 +655,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -657,15 +684,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -673,117 +700,150 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2019</v>
       </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>12.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>12.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+        <v>2019</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>2019</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -791,18 +851,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -816,26 +876,32 @@
       <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>23</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrected some required fields in schema and adapted tests accordingly
</commit_message>
<xml_diff>
--- a/financejson/tests/test.xlsx
+++ b/financejson/tests/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>symbol</t>
   </si>
@@ -65,6 +65,9 @@
     <t>period</t>
   </si>
   <si>
+    <t>2019-01-01</t>
+  </si>
+  <si>
     <t>+1q</t>
   </si>
   <si>
@@ -90,9 +93,6 @@
   </si>
   <si>
     <t>country</t>
-  </si>
-  <si>
-    <t>2019-01-01</t>
   </si>
   <si>
     <t>foo</t>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -783,81 +783,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -865,19 +797,102 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -885,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>

</xml_diff>